<commit_message>
reorder columns and update excel template
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -143,13 +143,62 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10001793525809276"/>
+          <c:y val="0.33119932925051038"/>
+          <c:w val="0.6780290901137358"/>
+          <c:h val="0.64767096821230674"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="10"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -167,6 +216,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -191,6 +241,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -215,6 +266,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -268,7 +320,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -322,10 +374,10 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>212</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>706</c:v>
+                  <c:v>712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,8 +398,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -376,7 +427,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -487,7 +538,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Arterial Switch</a:t>
+              <a:t>Redo Operations</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -522,26 +573,55 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="31750" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="17"/>
+          <c:explosion val="10"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -549,16 +629,72 @@
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
-          </c:marker>
-          <c:dLbls>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1AE2-444A-ACC6-741FE155D99D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
             <c:spPr>
-              <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1AE2-444A-ACC6-741FE155D99D}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -567,7 +703,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1"/>
                     </a:solidFill>
@@ -579,218 +715,79 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
+            <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
+            <c:separator>
+            </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:numRef>
-              <c:f>(Procedures!$A$766,Procedures!$A$851,Procedures!$A$936,Procedures!$A$1021,Procedures!$A$1106,Procedures!$A$1191,Procedures!$A$1276,Procedures!$A$1361,Procedures!$A$1446)</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+            <c:strRef>
+              <c:f>Redo!$A$50:$A$51</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2009</c:v>
+                  <c:v>First_Operation</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2017</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
+                  <c:v>Redo_Operation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Procedures!$F$793,Procedures!$F$878,Procedures!$F$963,Procedures!$F$1048,Procedures!$F$1133,Procedures!$F$1218,Procedures!$F$1303,Procedures!$F$1388,Procedures!$F$1473)</c:f>
+              <c:f>Redo!$N$50:$N$51</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>690</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>95</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4581-48E1-A5A0-E11814684928}"/>
+              <c16:uniqueId val="{00000004-1AE2-444A-ACC6-741FE155D99D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
+          <c:showPercent val="1"/>
           <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="754715760"/>
-        <c:axId val="754716744"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="754715760"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="754716744"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="754716744"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="95000"/>
-                      <a:lumOff val="5000"/>
-                      <a:alpha val="42000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                      <a:alpha val="36000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="754715760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -799,6 +796,42 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -894,355 +927,6 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Redo Operations</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="20000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000001-1AE2-444A-ACC6-741FE155D99D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="20000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-1AE2-444A-ACC6-741FE155D99D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:spPr>
-              <a:pattFill prst="pct75">
-                <a:fgClr>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:fgClr>
-                <a:bgClr>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:bgClr>
-              </a:pattFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:separator>
-            </c:separator>
-            <c:showLeaderLines val="1"/>
-            <c:leaderLines>
-              <c:spPr>
-                <a:ln w="9525">
-                  <a:solidFill>
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="50000"/>
-                      <a:lumOff val="50000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-            </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Redo!$A$50:$A$51</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>First_Operation</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Redo_Operation</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Redo!$N$50:$N$51</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>675</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>142</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-1AE2-444A-ACC6-741FE155D99D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="ctr"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="95000"/>
-            <a:alpha val="39000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:gradFill flip="none" rotWithShape="1">
-      <a:gsLst>
-        <a:gs pos="0">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="39000">
-          <a:schemeClr val="lt1"/>
-        </a:gs>
-        <a:gs pos="100000">
-          <a:schemeClr val="lt1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:gs>
-      </a:gsLst>
-      <a:path path="circle">
-        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-      </a:path>
-      <a:tileRect/>
-    </a:gradFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="25000"/>
-          <a:lumOff val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="dk1">
-                    <a:lumMod val="75000"/>
-                    <a:lumOff val="25000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
               <a:t>Residence</a:t>
             </a:r>
           </a:p>
@@ -1278,13 +962,52 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="10"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -1302,6 +1025,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1326,6 +1050,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1350,6 +1075,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1374,6 +1100,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1398,6 +1125,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -1451,7 +1179,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -1508,16 +1236,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>307</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>256</c:v>
+                  <c:v>259</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>237</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>22</c:v>
@@ -1541,8 +1269,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1571,7 +1298,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -1647,7 +1374,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1842,16 +1569,16 @@
                   <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>144</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>200</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>153</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2035,7 +1762,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2227,16 +1954,16 @@
                   <c:v>4.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.97</c:v>
+                  <c:v>3.89</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.68</c:v>
+                  <c:v>3.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.97</c:v>
+                  <c:v>3.99</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.75</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2.4300000000000002</c:v>
@@ -2423,7 +2150,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2644,7 +2371,7 @@
                   <c:v>268</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>307</c:v>
+                  <c:v>310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,7 +2557,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2908,13 +2635,52 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="10"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -2932,6 +2698,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -2956,6 +2723,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3057,10 +2825,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>413</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>576</c:v>
+                  <c:v>582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3081,8 +2849,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -3111,7 +2878,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -3127,6 +2894,410 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Arterial Switch</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>(Procedures!$A$757,Procedures!$A$841,Procedures!$A$925,Procedures!$A$1009,Procedures!$A$1093,Procedures!$A$1177,Procedures!$A$1261,Procedures!$A$1345,Procedures!$A$1429)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(Procedures!$F$784,Procedures!$F$868,Procedures!$F$952,Procedures!$F$1036,Procedures!$F$1120,Procedures!$F$1204,Procedures!$F$1288,Procedures!$F$1372,Procedures!$F$1456)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>95</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5384-48E5-B211-410D92C230A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="675991320"/>
+        <c:axId val="675992960"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="675991320"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="675992960"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="675992960"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="675991320"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3432,7 +3603,7 @@
                   <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>21</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3612,7 +3783,7 @@
                   <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>32</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3757,7 +3928,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -4054,7 +4225,7 @@
                   <c:v>806</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>989</c:v>
+                  <c:v>998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4717,13 +4888,52 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="10"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -4741,6 +4951,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4765,6 +4976,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4866,10 +5078,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>578</c:v>
+                  <c:v>584</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>411</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4890,8 +5102,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -4920,7 +5131,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -5188,10 +5399,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>19</c:v>
@@ -5460,13 +5671,52 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="10"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -5484,6 +5734,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5508,6 +5759,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5532,6 +5784,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5540,6 +5793,30 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-6.6666666666666666E-2"/>
+                  <c:y val="8.7962962962962965E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="bestFit"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="1"/>
+              <c:showBubbleSize val="0"/>
+              <c:separator>
+              </c:separator>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-7898-4875-BFEC-85BC297DD224}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:pattFill prst="pct75">
                 <a:fgClr>
@@ -5585,7 +5862,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="ctr"/>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
             <c:showCatName val="0"/>
@@ -5639,7 +5916,7 @@
                   <c:v>102</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24</c:v>
@@ -5663,8 +5940,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -5693,7 +5969,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -5832,13 +6108,52 @@
       </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="40"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
-      <c:pieChart>
+      <c:pie3DChart>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:explosion val="10"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
@@ -5856,6 +6171,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5880,6 +6196,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -5904,6 +6221,7 @@
                   </a:prstClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:sp3d/>
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -6034,7 +6352,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('2017'!$A$39,'2017'!$A$40,'2017'!$A$41)</c:f>
+              <c:f>('2017'!$A$38,'2017'!$A$39,'2017'!$A$40)</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -6051,12 +6369,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('2017'!$N$39,'2017'!$N$40,'2017'!$N$41)</c:f>
+              <c:f>('2017'!$N$38,'2017'!$N$39,'2017'!$N$40)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>79</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
@@ -6083,8 +6401,7 @@
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
+      </c:pie3DChart>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -6113,7 +6430,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1">
                   <a:lumMod val="75000"/>
@@ -7795,7 +8112,7 @@
 </file>
 
 <file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -7872,14 +8189,35 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -7889,15 +8227,29 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -7913,21 +8265,60 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
@@ -7942,50 +8333,9 @@
           <a:alpha val="85000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -8964,7 +9314,7 @@
 </file>
 
 <file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -9046,30 +9396,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -9079,29 +9406,15 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -9117,15 +9430,18 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -9139,15 +9455,18 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -10135,7 +10454,7 @@
 </file>
 
 <file path=xl/charts/style14.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="205">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10212,7 +10531,9 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
@@ -10302,9 +10623,7 @@
     <cs:spPr>
       <a:ln w="31750" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -10321,13 +10640,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -10705,7 +11022,7 @@
 </file>
 
 <file path=xl/charts/style15.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -10782,14 +11099,35 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -10799,15 +11137,29 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-          <a:alpha val="75000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -10823,21 +11175,60 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
@@ -10852,50 +11243,9 @@
           <a:alpha val="85000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="31750" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -11273,7 +11623,7 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="253">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -11350,35 +11700,14 @@
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -11388,29 +11717,15 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:pattFill prst="pct75">
-        <a:fgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:fgClr>
-        <a:bgClr>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:bgClr>
-      </a:pattFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="40000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
-    </cs:spPr>
-    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
       <a:spAutoFit/>
     </cs:bodyPr>
@@ -11426,15 +11741,18 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
@@ -11448,15 +11766,18 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr"/>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:effectLst>
-        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
-          <a:prstClr val="black">
-            <a:alpha val="20000"/>
-          </a:prstClr>
-        </a:outerShdw>
-      </a:effectLst>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
     </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
@@ -11471,9 +11792,7 @@
     <cs:spPr>
       <a:ln w="31750" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="85000"/>
-          </a:schemeClr>
+          <a:schemeClr val="phClr"/>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -11490,13 +11809,11 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:alpha val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="phClr"/>
       </a:solidFill>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -16868,44 +17185,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="13" name="Chart 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39434BE4-A803-47BE-BE9C-37BA36F08A51}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>81</xdr:row>
@@ -16936,7 +17215,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -16974,7 +17253,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17012,7 +17291,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17050,7 +17329,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17088,7 +17367,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -17113,6 +17392,44 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{430144E1-D853-4821-B59A-F51288028A50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B458B11-80C5-40F4-840F-091BF3CC78EE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>

<commit_message>
change template chart titles to reflect date
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Work\Audit\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11360B5EED8C10B1E0E014C0753BA3E310DFD234" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{175EC6FE-CFE1-4845-9A61-C4E298375697}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="11360B5EED8C10B1E0E014C0753BA3E310DFD234" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{86ECDF8C-6294-4783-BD60-7B2A93CD35BD}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -109,7 +109,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Age Groups</a:t>
+              <a:t>Pediatric Age Groups (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -598,7 +598,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Redo Operations</a:t>
+              <a:t>Redo Operations (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -781,6 +781,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-1AE2-444A-ACC6-741FE155D99D}"/>
                 </c:ext>
@@ -843,6 +844,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -1004,7 +1012,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Residence</a:t>
+              <a:t>Residence (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1293,6 +1301,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-44B0-4116-AFEB-BBB73A2BBD48}"/>
                 </c:ext>
@@ -1384,6 +1393,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-44B0-4116-AFEB-BBB73A2BBD48}"/>
                 </c:ext>
@@ -1425,6 +1435,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-44B0-4116-AFEB-BBB73A2BBD48}"/>
                 </c:ext>
@@ -1466,11 +1477,19 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-44B0-4116-AFEB-BBB73A2BBD48}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -1650,7 +1669,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Surgeons</a:t>
+              <a:t>Surgeons (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2092,7 +2111,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Week Days</a:t>
+              <a:t>Week Days (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3777,7 +3796,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Adults - Pediatrics</a:t>
+              <a:t>Adults - Pediatrics (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5489,7 +5508,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Gender</a:t>
+              <a:t>Gender (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5672,6 +5691,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-27F6-4D84-9B41-3580975F1377}"/>
                 </c:ext>
@@ -5713,11 +5733,19 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-27F6-4D84-9B41-3580975F1377}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -5879,7 +5907,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Aortic Surgery</a:t>
+              <a:t>Aortic Surgery (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -6327,11 +6355,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Mitral Valve Surgery</a:t>
+              <a:t>First-Time Mitral Valve Surgery (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16859038695002387"/>
+          <c:y val="2.7500000902231002E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6596,6 +6632,7 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-7898-4875-BFEC-85BC297DD224}"/>
                 </c:ext>
@@ -6637,11 +6674,19 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-7898-4875-BFEC-85BC297DD224}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -6802,7 +6847,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Tricuspid Valve Surgery</a:t>
+              <a:t>Tricuspid Valve Surgery (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7162,6 +7207,13 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
@@ -7329,7 +7381,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>TGA</a:t>
+              <a:t>TGA (2017)</a:t>
             </a:r>
           </a:p>
         </c:rich>

</xml_diff>

<commit_message>
Add Mortality data to totals
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,7 +8,6 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Work\Audit\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="11360B5EED8C10B1E0E014C0753BA3E310DFD234" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{856E5E00-32FB-477B-9041-9883E1692974}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,7 +251,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>(Totals!$A$1,Totals!$A$5,Totals!$A$9,Totals!$A$13,Totals!$A$17,Totals!$A$21,Totals!$A$25,Totals!$A$29,Totals!$A$33)</c:f>
+              <c:f>(Totals!$A$1,Totals!$A$7,Totals!$A$13,Totals!$A$19,Totals!$A$25,Totals!$A$31,Totals!$A$37,Totals!$A$43,Totals!$A$49)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -288,7 +287,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Totals!$N$2,Totals!$N$6,Totals!$N$10,Totals!$N$14,Totals!$N$18,Totals!$N$22,Totals!$N$26,Totals!$N$30,Totals!$N$34)</c:f>
+              <c:f>(Totals!$N$2,Totals!$N$8,Totals!$N$14,Totals!$N$20,Totals!$N$26,Totals!$N$32,Totals!$N$38,Totals!$N$44,Totals!$N$50)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -317,7 +316,7 @@
                   <c:v>809</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1002</c:v>
+                  <c:v>1009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -837,7 +836,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>693</c:v>
+                  <c:v>694</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>144</c:v>
@@ -1125,28 +1124,28 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>73</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>122</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>71</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>102</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1291,31 +1290,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>57</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>29</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1469,22 +1468,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>24</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>24</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2288,7 +2287,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>312</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>259</c:v>
@@ -2297,10 +2296,10 @@
                   <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>240</c:v>
+                  <c:v>241</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2614,7 +2613,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.89</c:v>
+                  <c:v>3.88</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4.0199999999999996</c:v>
@@ -3037,7 +3036,7 @@
                   <c:v>269</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>312</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3430,7 +3429,7 @@
                   <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.89</c:v>
+                  <c:v>3.88</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4221,7 +4220,7 @@
                   <c:v>18.309999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.740000000000002</c:v>
+                  <c:v>22.73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5668,7 +5667,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('2017'!$A$26,'2017'!$A$27,'2017'!$A$28,'2017'!$A$29,'2017'!$A$30,'2017'!$A$31,'2017'!$A$33,'2017'!$A$34)</c:f>
+              <c:f>('2017'!$A$28,'2017'!$A$29,'2017'!$A$30,'2017'!$A$31,'2017'!$A$32,'2017'!$A$33,'2017'!$A$35,'2017'!$A$36)</c:f>
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
@@ -5700,7 +5699,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('2017'!$N$26,'2017'!$N$27,'2017'!$N$28,'2017'!$N$29,'2017'!$N$30,'2017'!$N$31,'2017'!$N$33,'2017'!$N$34)</c:f>
+              <c:f>('2017'!$N$28,'2017'!$N$29,'2017'!$N$30,'2017'!$N$31,'2017'!$N$32,'2017'!$N$33,'2017'!$N$35,'2017'!$N$36)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6116,7 +6115,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('2017'!$A$52,'2017'!$A$53,'2017'!$A$56)</c:f>
+              <c:f>('2017'!$A$54,'2017'!$A$55,'2017'!$A$58)</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -6133,7 +6132,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('2017'!$N$52,'2017'!$N$53,'2017'!$N$56)</c:f>
+              <c:f>('2017'!$N$54,'2017'!$N$55,'2017'!$N$58)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -7088,7 +7087,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>(Totals!$A$1,Totals!$A$5,Totals!$A$9,Totals!$A$13,Totals!$A$17,Totals!$A$21,Totals!$A$25,Totals!$A$29,Totals!$A$33)</c:f>
+              <c:f>(Totals!$A$1,Totals!$A$7,Totals!$A$13,Totals!$A$19,Totals!$A$25,Totals!$A$31,Totals!$A$37,Totals!$A$43,Totals!$A$49)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7124,7 +7123,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Totals!$O$2,Totals!$O$6,Totals!$O$10,Totals!$O$14,Totals!$O$18,Totals!$O$22,Totals!$O$26,Totals!$O$30,Totals!$O$34)</c:f>
+              <c:f>(Totals!$O$2,Totals!$O$8,Totals!$O$14,Totals!$O$20,Totals!$O$26,Totals!$O$32,Totals!$O$38,Totals!$O$44,Totals!$O$50)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -7153,7 +7152,7 @@
                   <c:v>67.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>83.5</c:v>
+                  <c:v>84.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7596,10 +7595,10 @@
                   <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>144</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>204</c:v>
@@ -7608,7 +7607,7 @@
                   <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8050,6 +8049,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9481174042047779E-2"/>
+                  <c:y val="2.2916667418525813E-2"/>
+                </c:manualLayout>
+              </c:layout>
               <c:spPr>
                 <a:noFill/>
                 <a:ln>
@@ -8059,7 +8064,7 @@
               </c:spPr>
               <c:txPr>
                 <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
+                  <a:noAutofit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
@@ -8076,7 +8081,7 @@
                   <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
-              <c:dLblPos val="outEnd"/>
+              <c:dLblPos val="bestFit"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="1"/>
@@ -8084,7 +8089,14 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.2186066030004076"/>
+                      <c:h val="0.19625833977225524"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-78D5-40C6-9209-FA18EB2F1AE8}"/>
                 </c:ext>
@@ -8101,7 +8113,7 @@
               </c:spPr>
               <c:txPr>
                 <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
+                  <a:noAutofit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
@@ -8126,7 +8138,14 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.21315187426863416"/>
+                      <c:h val="0.20084167325596042"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-78D5-40C6-9209-FA18EB2F1AE8}"/>
                 </c:ext>
@@ -8136,8 +8155,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-8.9056795620789872E-2"/>
-                  <c:y val="-4.5833334837051664E-3"/>
+                  <c:x val="-6.6792706283500383E-2"/>
+                  <c:y val="-3.4375001127788752E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:spPr>
@@ -8149,7 +8168,7 @@
               </c:spPr>
               <c:txPr>
                 <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                  <a:spAutoFit/>
+                  <a:noAutofit/>
                 </a:bodyPr>
                 <a:lstStyle/>
                 <a:p>
@@ -8174,7 +8193,14 @@
               <c:showPercent val="1"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.23902019993951845"/>
+                      <c:h val="0.19396631213800236"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-78D5-40C6-9209-FA18EB2F1AE8}"/>
                 </c:ext>
@@ -8261,22 +8287,22 @@
             <c:strLit>
               <c:ptCount val="4"/>
               <c:pt idx="0">
-                <c:v>&lt;1m</c:v>
+                <c:v>Neonates (&lt;1m)</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v> 1m-1yr</c:v>
+                <c:v>Infants (1m-1yr)</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v> 1yr-2yr</c:v>
+                <c:v>Toddlers (1yr-2yr)</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v> &gt;2r</c:v>
+                <c:v>Children (&gt;2r)</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2017'!$N$12:$N$15</c:f>
+              <c:f>'2017'!$N$14:$N$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -8284,13 +8310,13 @@
                   <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>215</c:v>
+                  <c:v>217</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>219</c:v>
+                  <c:v>221</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8445,7 +8471,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2017'!$A$6</c:f>
+              <c:f>'2017'!$A$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8553,47 +8579,43 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'2017'!$B$5:$M$5</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'2017'!$C$5:$M$5</c:f>
+              <c:f>'2017'!$B$7:$M$7</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>FEB</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>MAR</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>APR</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>MAY</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>JUN</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>JUL</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>AUG</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>SEP</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>OCT</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>NOV</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>DEC</c:v>
                 </c:pt>
               </c:strCache>
@@ -8601,34 +8623,27 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'2017'!$B$6:$M$6</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'2017'!$C$6:$M$6</c:f>
+              <c:f>'2017'!$B$8:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>33</c:v>
@@ -8637,13 +8652,16 @@
                   <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>24</c:v>
+                <c:pt idx="11">
+                  <c:v>27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8659,7 +8677,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2017'!$A$7</c:f>
+              <c:f>'2017'!$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8767,47 +8785,43 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'2017'!$B$5:$M$5</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'2017'!$C$5:$M$5</c:f>
+              <c:f>'2017'!$B$7:$M$7</c:f>
               <c:strCache>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>FEB</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>MAR</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>APR</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>MAY</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>JUN</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>JUL</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>AUG</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>SEP</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>OCT</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>NOV</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>DEC</c:v>
                 </c:pt>
               </c:strCache>
@@ -8815,49 +8829,45 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'2017'!$B$7:$M$7</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'2017'!$C$7:$M$7</c:f>
+              <c:f>'2017'!$B$9:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>46</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>56</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>49</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>62</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>39</c:v>
+                <c:pt idx="11">
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8890,7 +8900,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'2017'!$A$8</c:f>
+              <c:f>'2017'!$A$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9003,92 +9013,86 @@
           </c:dLbls>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="12"/>
+              <c:ptCount val="13"/>
               <c:pt idx="0">
+                <c:v>JAN</c:v>
+              </c:pt>
+              <c:pt idx="1">
                 <c:v>FEB</c:v>
               </c:pt>
-              <c:pt idx="1">
+              <c:pt idx="2">
                 <c:v>MAR</c:v>
               </c:pt>
-              <c:pt idx="2">
+              <c:pt idx="3">
                 <c:v>APR</c:v>
               </c:pt>
-              <c:pt idx="3">
+              <c:pt idx="4">
                 <c:v>MAY</c:v>
               </c:pt>
-              <c:pt idx="4">
+              <c:pt idx="5">
                 <c:v>JUN</c:v>
               </c:pt>
-              <c:pt idx="5">
+              <c:pt idx="6">
                 <c:v>JUL</c:v>
               </c:pt>
-              <c:pt idx="6">
+              <c:pt idx="7">
                 <c:v>AUG</c:v>
               </c:pt>
-              <c:pt idx="7">
+              <c:pt idx="8">
                 <c:v>SEP</c:v>
               </c:pt>
-              <c:pt idx="8">
+              <c:pt idx="9">
                 <c:v>OCT</c:v>
               </c:pt>
-              <c:pt idx="9">
+              <c:pt idx="10">
                 <c:v>NOV</c:v>
               </c:pt>
-              <c:pt idx="10">
+              <c:pt idx="11">
                 <c:v>DEC</c:v>
               </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>'2017'!$B$8:$M$8</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'2017'!$C$8:$M$8</c:f>
+              <c:f>'2017'!$B$10:$M$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>95</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
                   <c:v>87</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>77</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>91</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>67</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>89</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>82</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>97</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>84</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>63</c:v>
+                <c:pt idx="11">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9246,6 +9250,16 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="11"/>
+              <c:delete val="1"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-CA27-4810-A1DB-EAAA249DF813}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -9284,80 +9298,57 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="12"/>
+              <c:ptCount val="13"/>
               <c:pt idx="0">
+                <c:v>JAN</c:v>
+              </c:pt>
+              <c:pt idx="1">
                 <c:v>FEB</c:v>
               </c:pt>
-              <c:pt idx="1">
+              <c:pt idx="2">
                 <c:v>MAR</c:v>
               </c:pt>
-              <c:pt idx="2">
+              <c:pt idx="3">
                 <c:v>APR</c:v>
               </c:pt>
-              <c:pt idx="3">
+              <c:pt idx="4">
                 <c:v>MAY</c:v>
               </c:pt>
-              <c:pt idx="4">
+              <c:pt idx="5">
                 <c:v>JUN</c:v>
               </c:pt>
-              <c:pt idx="5">
+              <c:pt idx="6">
                 <c:v>JUL</c:v>
               </c:pt>
-              <c:pt idx="6">
+              <c:pt idx="7">
                 <c:v>AUG</c:v>
               </c:pt>
-              <c:pt idx="7">
+              <c:pt idx="8">
                 <c:v>SEP</c:v>
               </c:pt>
-              <c:pt idx="8">
+              <c:pt idx="9">
                 <c:v>OCT</c:v>
               </c:pt>
-              <c:pt idx="9">
+              <c:pt idx="10">
                 <c:v>NOV</c:v>
               </c:pt>
-              <c:pt idx="10">
+              <c:pt idx="11">
                 <c:v>DEC</c:v>
               </c:pt>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:autoCat val="1"/>
-                </c:ext>
-              </c:extLst>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>(Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6)</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>(Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6)</c:f>
+              <c:f>(Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6,Charts!$S$6)</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>56.116666666666674</c:v>
                 </c:pt>
@@ -9392,6 +9383,9 @@
                   <c:v>56.116666666666674</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>56.116666666666674</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>56.116666666666674</c:v>
                 </c:pt>
               </c:numCache>
@@ -9918,7 +9912,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2017'!$A$6:$A$7</c:f>
+              <c:f>'2017'!$A$8:$A$9</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -9932,15 +9926,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2017'!$N$6:$N$7</c:f>
+              <c:f>'2017'!$N$8:$N$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>417</c:v>
+                  <c:v>420</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>585</c:v>
+                  <c:v>589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10317,7 +10311,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2017'!$A$20:$A$21</c:f>
+              <c:f>'2017'!$A$22:$A$23</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -10331,15 +10325,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2017'!$N$20:$N$21</c:f>
+              <c:f>'2017'!$N$22:$N$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>587</c:v>
+                  <c:v>593</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>415</c:v>
+                  <c:v>416</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11250,13 +11244,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>102</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11755,7 +11749,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'2017'!$A$39:$A$41</c:f>
+              <c:f>'2017'!$A$41:$A$43</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -11772,15 +11766,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2017'!$N$39:$N$41</c:f>
+              <c:f>'2017'!$N$41:$N$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -23740,8 +23734,8 @@
         <v>1</v>
       </c>
       <c r="S2" s="0">
-        <f>SUM(Totals!$N$2,Totals!$N$6,Totals!$N$10,Totals!$N$14,Totals!$N$18,Totals!$N$22,Totals!$N$26,Totals!$N$30,Totals!$N$34)</f>
-        <v>5230</v>
+        <f>SUM(Totals!N2,Totals!N8,Totals!N14,Totals!N20,Totals!N26,Totals!N32,Totals!N38,Totals!N44,Totals!N50)</f>
+        <v>5237</v>
       </c>
     </row>
     <row r="4">
@@ -23749,8 +23743,8 @@
         <v>2</v>
       </c>
       <c r="S4" s="1">
-        <f>AVERAGE(Totals!$O$2,Totals!$O$6,Totals!$O$10,Totals!$O$14,Totals!$O$18,Totals!$O$22,Totals!$O$26,Totals!$O$30,Totals!$O$34)</f>
-        <v>48.43333333333333</v>
+        <f>AVERAGE(Totals!O2,Totals!O8,Totals!O14,Totals!O20,Totals!O26,Totals!O32,Totals!O38,Totals!O44,Totals!O50)</f>
+        <v>48.5</v>
       </c>
     </row>
     <row r="6">
@@ -23758,7 +23752,7 @@
         <v>3</v>
       </c>
       <c r="S6" s="1">
-        <f>AVERAGE(Totals!$O$10,Totals!$O$14,Totals!$O$18,Totals!$O$22,Totals!$O$26,Totals!$O$30)</f>
+        <f>AVERAGE(Totals!O14,Totals!O20,Totals!O26,Totals!O32,Totals!O38,Totals!O44)</f>
         <v>56.116666666666674</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add length of stay
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Work\Audit\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="151" documentId="FC91A5086B230B3FBF10FC09D7C71FA5B6A8F71D" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{B0744990-CADA-4FDA-B94B-A5A293DB9F69}"/>
+  <xr:revisionPtr revIDLastSave="217" documentId="FC91A5086B230B3FBF10FC09D7C71FA5B6A8F71D" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{0725FD4E-8D14-4227-AB3C-EB1680D06314}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13128" windowHeight="6108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10206" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10241" uniqueCount="465">
   <si>
     <t xml:space="preserve">                               </t>
   </si>
@@ -1397,6 +1397,24 @@
   </si>
   <si>
     <t>Total/Surgeon (2018)</t>
+  </si>
+  <si>
+    <t>Total.pre</t>
+  </si>
+  <si>
+    <t>Total.post</t>
+  </si>
+  <si>
+    <t>Adults.pre</t>
+  </si>
+  <si>
+    <t>Adults.post</t>
+  </si>
+  <si>
+    <t>Pediatrics.pre</t>
+  </si>
+  <si>
+    <t>Pediatrics.post</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1424,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="151" x14ac:knownFonts="1">
+  <fonts count="153" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -2215,6 +2233,16 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="50">
     <fill>
@@ -2524,7 +2552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2975,6 +3003,12 @@
     <xf numFmtId="0" fontId="150" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="152" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3219,7 +3253,7 @@
                   <c:v>1015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>267</c:v>
+                  <c:v>513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3643,7 +3677,7 @@
                   <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4042,7 +4076,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5076,7 +5110,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6754,28 +6788,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7187,13 +7221,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7611,7 +7645,7 @@
                   <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7780,7 +7814,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7947,7 +7981,7 @@
                   <c:v>116</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8389,22 +8423,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>19</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8800,25 +8834,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>31</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37</c:v>
+                  <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9248,7 +9282,7 @@
                   <c:v>1015</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>267</c:v>
+                  <c:v>513</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9429,10 +9463,10 @@
                   <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>46</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9611,10 +9645,10 @@
                   <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.5</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.7</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10090,7 +10124,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10254,10 +10288,10 @@
                   <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.7</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10708,7 +10742,7 @@
                   <c:v>85</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10940,7 +10974,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Adults/Peds Mortality Percentage (2017)</a:t>
+              <a:t>Adults/Peds Mortality Percentage (2018)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -11104,10 +11138,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>111</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11276,10 +11310,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.7</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11749,7 +11783,7 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11878,7 +11912,7 @@
                   <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12001,7 +12035,7 @@
                   <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12107,10 +12141,10 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.7</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.8</c:v>
+                  <c:v>1.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12599,25 +12633,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12764,25 +12798,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12953,25 +12987,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>32</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13396,16 +13430,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>73</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13549,13 +13583,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13697,16 +13731,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44</c:v>
+                  <c:v>98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14405,13 +14439,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14815,10 +14849,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>111</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15106,7 +15140,7 @@
                   <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -15261,7 +15295,7 @@
                   <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -15421,7 +15455,7 @@
                   <c:v>267</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>513</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -15522,7 +15556,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{726B2B82-43C4-4ACD-8E49-88B2E056FE97}" type="CELLRANGE">
+                    <a:fld id="{3A52DB61-6746-4197-9E99-DAE4937805CD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -16566,16 +16600,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>56</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16876,7 +16910,7 @@
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17395,10 +17429,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>165</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>102</c:v>
+                  <c:v>198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17716,13 +17750,13 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -17919,13 +17953,13 @@
                   <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -18144,13 +18178,13 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -18888,6 +18922,1463 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="758061104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart30.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Length of Hospital Stay (2018)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:alpha val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="31750" cap="rnd" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="circle"/>
+          <c:size val="17"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Length of Stay'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adults-Peds'!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Length of Stay'!$D$2:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B379-45E5-9623-BD23953E1482}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Pre-op</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adults-Peds'!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Length of Stay'!$E$2:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B379-45E5-9623-BD23953E1482}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Post-op</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adults-Peds'!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Length of Stay'!$F$2:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B379-45E5-9623-BD23953E1482}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="862875064"/>
+        <c:axId val="862879000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="862875064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="862879000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="862879000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="862875064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart31.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Length</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> of Hospital Stay (Adults vs Peds)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Length of Stay'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Adults</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adults-Peds'!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Length of Stay'!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0F50-4AB8-BBA9-6A3BE42B376C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Length of Stay'!$J$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Pediatrics</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Adults-Peds'!$B$1:$M$1</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>JAN</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FEB</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MAR</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>APR</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MAY</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>JUN</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>JUL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>AUG</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>SEP</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>OCT</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>NOV</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>DEC</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Length of Stay'!$J$2:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0F50-4AB8-BBA9-6A3BE42B376C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="763600912"/>
+        <c:axId val="763598288"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="763600912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763598288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="763598288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="763600912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -19393,13 +20884,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>14</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19920,13 +21411,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20323,10 +21814,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>163</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20634,7 +22125,7 @@
                   <c:v>94</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20803,7 +22294,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20972,7 +22463,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21178,7 +22669,7 @@
                   <c:v>131</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21981,19 +23472,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>174</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>109</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -22307,7 +23798,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -23309,6 +24800,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -33943,6 +35514,1010 @@
         <a:noFill/>
       </a:ln>
     </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style28.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style29.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="342">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -38751,6 +41326,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>225</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>100060</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>157018</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="35" name="Chart 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74AED6F2-12E8-4E42-B9A6-AE1CCB336574}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>241</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>100060</xdr:colOff>
+      <xdr:row>255</xdr:row>
+      <xdr:rowOff>157018</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="36" name="Chart 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{019DF6B7-F074-4564-A04A-A843510D3980}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -39077,7 +41728,7 @@
       </c>
       <c r="S2">
         <f>SUM(Totals!N2,Totals!N8,Totals!N14,Totals!N20,Totals!N26,Totals!N32,Totals!N38,Totals!N44,Totals!N50,Totals!N56)</f>
-        <v>5502</v>
+        <v>5748</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -39094,7 +41745,7 @@
       </c>
       <c r="S4" s="1">
         <f>ROUND(AVERAGE(Totals!O2,Totals!O8,Totals!O14,Totals!O20,Totals!O26,Totals!O32,Totals!O38,Totals!O44,Totals!O50,Totals!O56), 1)</f>
-        <v>55.5</v>
+        <v>55.2</v>
       </c>
       <c r="W4">
         <v>2009</v>
@@ -39192,7 +41843,7 @@
         <v>3</v>
       </c>
       <c r="S10">
-        <v>267</v>
+        <v>513</v>
       </c>
       <c r="W10">
         <v>2015</v>
@@ -39225,7 +41876,7 @@
       </c>
       <c r="S12">
         <f>SUM(Totals!N3,Totals!N9,Totals!N15,Totals!N21,Totals!N27,Totals!N33,Totals!N39,Totals!N45,Totals!N51,Totals!N57)</f>
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="W12">
         <v>2017</v>
@@ -39245,11 +41896,11 @@
       </c>
       <c r="X13">
         <f>SUM(Procedures!$N$937,Procedures!$N$938)</f>
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="Z13">
         <f>SUM('Non-redo Procedures'!$F$921,'Non-redo Procedures'!$F$922,'Non-redo Procedures'!$F$923)</f>
-        <v>24</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -39258,7 +41909,7 @@
       </c>
       <c r="S14">
         <f>ROUND(AVERAGE(Totals!O3,Totals!O9,Totals!O15,Totals!O21,Totals!O27,Totals!O33,Totals!O39,Totals!O45,Totals!O51,Totals!O57), 1)</f>
-        <v>3</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -39276,7 +41927,7 @@
       </c>
       <c r="S18">
         <f>ROUND(AVERAGE(Totals!N4,Totals!N10,Totals!N16,Totals!N22,Totals!N28,Totals!N34,Totals!N40,Totals!N46,Totals!N52,Totals!N58),1)</f>
-        <v>4.5999999999999996</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="18:24" x14ac:dyDescent="0.55000000000000004">
@@ -39299,7 +41950,7 @@
       </c>
       <c r="X29">
         <f>SUM(Surgeons!$N$92,Trainers!$N$74)</f>
-        <v>20</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="18:24" x14ac:dyDescent="0.55000000000000004">
@@ -39308,7 +41959,7 @@
       </c>
       <c r="X30">
         <f>SUM(Surgeons!$N$93,Trainers!$N$75)</f>
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="18:24" x14ac:dyDescent="0.55000000000000004">
@@ -39317,7 +41968,7 @@
       </c>
       <c r="X31">
         <f>SUM(Surgeons!$N$94,Trainers!$N$76)</f>
-        <v>44</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="18:24" x14ac:dyDescent="0.55000000000000004">
@@ -39326,7 +41977,7 @@
       </c>
       <c r="X32">
         <f>SUM(Surgeons!$N$95,Trainers!$N$77)</f>
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="33" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39335,7 +41986,7 @@
       </c>
       <c r="X33">
         <f>SUM(Surgeons!$N$96,Trainers!$N$78)</f>
-        <v>44</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39357,14 +42008,14 @@
       </c>
       <c r="X45">
         <f>SUM('Adult Procedures'!$F911:$F920)</f>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="AA45" t="s">
         <v>195</v>
       </c>
       <c r="AB45">
         <f>SUM('Pediatric Procedures'!$F961)</f>
-        <v>31</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39373,14 +42024,14 @@
       </c>
       <c r="X46">
         <f>SUM('Adult Procedures'!$F921:$F923)</f>
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="AA46" t="s">
         <v>189</v>
       </c>
       <c r="AB46">
         <f>SUM('Pediatric Procedures'!$F911:$F926)</f>
-        <v>18</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39389,14 +42040,14 @@
       </c>
       <c r="X47">
         <f>SUM('Adult Procedures'!$F928:$F929)</f>
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="AA47" t="s">
         <v>190</v>
       </c>
       <c r="AB47">
         <f>SUM('Pediatric Procedures'!$F937:$F941)</f>
-        <v>28</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39405,14 +42056,14 @@
       </c>
       <c r="X48">
         <f>SUM('Adult Procedures'!$F930)</f>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="AA48" t="s">
         <v>191</v>
       </c>
       <c r="AB48">
         <f>SUM('Pediatric Procedures'!$F946:$F948)</f>
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39421,14 +42072,14 @@
       </c>
       <c r="X49">
         <f>SUM('Adult Procedures'!$F937:$F985)</f>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="AA49" t="s">
         <v>192</v>
       </c>
       <c r="AB49">
         <f>SUM('Pediatric Procedures'!$F958:$F960)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39437,14 +42088,14 @@
       </c>
       <c r="X50">
         <f>SUM('Adult Procedures'!F924:F927,'Adult Procedures'!F932:F936)</f>
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="AA50" t="s">
         <v>193</v>
       </c>
       <c r="AB50">
         <f>SUM('Pediatric Procedures'!$F962:$F972)</f>
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="23:28" x14ac:dyDescent="0.55000000000000004">
@@ -39453,7 +42104,7 @@
       </c>
       <c r="AB51">
         <f>SUM('Pediatric Procedures'!$F978:$F985)</f>
-        <v>32</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>